<commit_message>
adjustments to ratings display
</commit_message>
<xml_diff>
--- a/app/adp/templates/template.xlsx
+++ b/app/adp/templates/template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\carboni\sca-scratchspace\adp-program-reformat\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\carboni\projects\shupe-carboni\backend\app\adp\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AF08B5D-E8DD-43D0-8665-46DBB9FF3F8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7711AB6D-BD0F-40C7-BE17-B2E76E177D91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2280" yWindow="3345" windowWidth="23430" windowHeight="15345" tabRatio="856" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" tabRatio="856" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="9-col" sheetId="2" r:id="rId1"/>
@@ -38,12 +38,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="19">
   <si>
     <t>Confidential Pricing</t>
-  </si>
-  <si>
-    <t>AHRI Ratings</t>
   </si>
   <si>
     <t>AHRINumber</t>
@@ -82,12 +79,6 @@
     <t>MODEL</t>
   </si>
   <si>
-    <t>Parts Pricing</t>
-  </si>
-  <si>
-    <t>All Parts</t>
-  </si>
-  <si>
     <t>Part Number</t>
   </si>
   <si>
@@ -101,6 +92,9 @@
   </si>
   <si>
     <t>Nomenclature</t>
+  </si>
+  <si>
+    <t>Field Installed Accessories</t>
   </si>
 </sst>
 </file>
@@ -747,7 +741,7 @@
     <xf numFmtId="44" fontId="20" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="20" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -813,6 +807,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -825,7 +828,6 @@
     <xf numFmtId="0" fontId="19" fillId="33" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="46">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -897,14 +899,14 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>25129</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>234679</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>51435</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>477927</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>487452</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>36195</xdr:rowOff>
     </xdr:to>
@@ -929,7 +931,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3206479" y="241935"/>
+          <a:off x="3901804" y="241935"/>
           <a:ext cx="2576873" cy="1318260"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1077,104 +1079,6 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3654154" y="289560"/>
-          <a:ext cx="2576873" cy="1318260"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>63229</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>184785</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>2640102</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>169545</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1A33D1A0-1B80-4F8C-BB64-2C20F680EACD}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3101704" y="184785"/>
-          <a:ext cx="2576873" cy="1318260"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>1053829</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>80010</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>811302</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>64770</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7CF23A07-14A4-425A-9F52-4BDA507C40D7}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3597004" y="270510"/>
           <a:ext cx="2576873" cy="1318260"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1487,14 +1391,14 @@
   <dimension ref="A10:R15"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.140625" customWidth="1"/>
-    <col min="3" max="6" width="8" customWidth="1"/>
+    <col min="1" max="1" width="34.5703125" customWidth="1"/>
+    <col min="2" max="2" width="20.42578125" customWidth="1"/>
+    <col min="3" max="6" width="8.7109375" customWidth="1"/>
     <col min="7" max="7" width="15.85546875" customWidth="1"/>
     <col min="8" max="8" width="36.85546875" customWidth="1"/>
     <col min="9" max="9" width="14.85546875" bestFit="1" customWidth="1"/>
@@ -1504,29 +1408,29 @@
   </cols>
   <sheetData>
     <row r="10" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A10" s="23" t="s">
+      <c r="A10" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="23"/>
-      <c r="C10" s="23"/>
-      <c r="D10" s="23"/>
-      <c r="E10" s="23"/>
-      <c r="F10" s="23"/>
-      <c r="G10" s="23"/>
-      <c r="H10" s="23"/>
-      <c r="I10" s="23"/>
+      <c r="B10" s="26"/>
+      <c r="C10" s="26"/>
+      <c r="D10" s="26"/>
+      <c r="E10" s="26"/>
+      <c r="F10" s="26"/>
+      <c r="G10" s="26"/>
+      <c r="H10" s="26"/>
+      <c r="I10" s="26"/>
     </row>
     <row r="11" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="12" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A12" s="24"/>
-      <c r="B12" s="25"/>
-      <c r="C12" s="25"/>
-      <c r="D12" s="25"/>
-      <c r="E12" s="25"/>
-      <c r="F12" s="25"/>
-      <c r="G12" s="25"/>
-      <c r="H12" s="25"/>
-      <c r="I12" s="26"/>
+      <c r="A12" s="27"/>
+      <c r="B12" s="28"/>
+      <c r="C12" s="28"/>
+      <c r="D12" s="28"/>
+      <c r="E12" s="28"/>
+      <c r="F12" s="28"/>
+      <c r="G12" s="28"/>
+      <c r="H12" s="28"/>
+      <c r="I12" s="29"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
@@ -1578,26 +1482,26 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88BD92AB-7931-43E7-91D7-E5F4C81157E3}">
-  <dimension ref="B10:R10"/>
+  <dimension ref="B10:J10"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="10" spans="2:10" ht="21" x14ac:dyDescent="0.35">
-      <c r="B10" s="23" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" s="23"/>
-      <c r="D10" s="23"/>
-      <c r="E10" s="23"/>
-      <c r="F10" s="23"/>
-      <c r="G10" s="23"/>
-      <c r="H10" s="23"/>
-      <c r="I10" s="23"/>
-      <c r="J10" s="23"/>
+      <c r="B10" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="26"/>
+      <c r="D10" s="26"/>
+      <c r="E10" s="26"/>
+      <c r="F10" s="26"/>
+      <c r="G10" s="26"/>
+      <c r="H10" s="26"/>
+      <c r="I10" s="26"/>
+      <c r="J10" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1615,7 +1519,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{856AC59C-B913-4AAB-AD67-AEC6500AAAE2}">
-  <dimension ref="B10:R10"/>
+  <dimension ref="B10:K10"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B16" sqref="B16"/>
@@ -1624,18 +1528,18 @@
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="10" spans="2:11" ht="21" x14ac:dyDescent="0.35">
-      <c r="B10" s="23" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" s="23"/>
-      <c r="D10" s="23"/>
-      <c r="E10" s="23"/>
-      <c r="F10" s="23"/>
-      <c r="G10" s="23"/>
-      <c r="H10" s="23"/>
-      <c r="I10" s="27"/>
-      <c r="J10" s="27"/>
-      <c r="K10" s="27"/>
+      <c r="B10" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="26"/>
+      <c r="D10" s="26"/>
+      <c r="E10" s="26"/>
+      <c r="F10" s="26"/>
+      <c r="G10" s="26"/>
+      <c r="H10" s="26"/>
+      <c r="I10" s="22"/>
+      <c r="J10" s="22"/>
+      <c r="K10" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1653,7 +1557,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{790636CD-455E-4A76-AE4D-0E945794E185}">
-  <dimension ref="B10:R10"/>
+  <dimension ref="B10:J10"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B10" sqref="B10:F10"/>
@@ -1662,17 +1566,17 @@
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="10" spans="2:10" ht="21" x14ac:dyDescent="0.35">
-      <c r="B10" s="23" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" s="23"/>
-      <c r="D10" s="23"/>
-      <c r="E10" s="23"/>
-      <c r="F10" s="23"/>
-      <c r="G10" s="27"/>
-      <c r="H10" s="27"/>
-      <c r="I10" s="27"/>
-      <c r="J10" s="27"/>
+      <c r="B10" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="26"/>
+      <c r="D10" s="26"/>
+      <c r="E10" s="26"/>
+      <c r="F10" s="26"/>
+      <c r="G10" s="22"/>
+      <c r="H10" s="22"/>
+      <c r="I10" s="22"/>
+      <c r="J10" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1690,89 +1594,73 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73B9B48C-6839-420E-9C83-013064823206}">
-  <dimension ref="B10:M15"/>
+  <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.7109375" customWidth="1"/>
-    <col min="3" max="3" width="47" customWidth="1"/>
-    <col min="4" max="4" width="9.7109375" customWidth="1"/>
-    <col min="5" max="5" width="12.140625" customWidth="1"/>
-    <col min="6" max="6" width="18.5703125" customWidth="1"/>
-    <col min="7" max="12" width="9.140625" customWidth="1"/>
-    <col min="13" max="13" width="9.140625" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="0" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="30.85546875" customWidth="1"/>
+    <col min="2" max="2" width="26.42578125" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" customWidth="1"/>
+    <col min="5" max="5" width="18.5703125" customWidth="1"/>
+    <col min="6" max="11" width="9.140625" customWidth="1"/>
+    <col min="12" max="13" width="9.140625" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="10" spans="2:7" ht="21" x14ac:dyDescent="0.35">
-      <c r="B10" s="23" t="s">
+    <row r="1" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="29"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="23"/>
-      <c r="D10" s="23"/>
-      <c r="E10" s="23"/>
-      <c r="G10" s="22"/>
+      <c r="B2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="11" spans="2:7" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="G11" s="22"/>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="24"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="6"/>
     </row>
-    <row r="12" spans="2:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B12" s="24" t="s">
-        <v>15</v>
-      </c>
-      <c r="C12" s="25"/>
-      <c r="D12" s="25"/>
-      <c r="E12" s="26"/>
-    </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B13" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B14" s="4"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="6"/>
-    </row>
-    <row r="15" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="7"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="10"/>
+    <row r="4" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="25"/>
+      <c r="B4" s="23"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="10"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="B10:E10"/>
+  <mergeCells count="1">
+    <mergeCell ref="A1:D1"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.2" right="0.2" top="0.5" bottom="0.25" header="0.05" footer="0.05"/>
   <pageSetup orientation="landscape" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{757B66A0-E2C7-4672-9A91-343D1A4BCA06}">
-  <dimension ref="A10:R15"/>
+  <dimension ref="A1:R4"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:H1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1782,156 +1670,136 @@
     <col min="3" max="3" width="20.28515625" customWidth="1"/>
     <col min="4" max="4" width="22" customWidth="1"/>
     <col min="5" max="5" width="26.42578125" customWidth="1"/>
-    <col min="6" max="6" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="11.28515625" customWidth="1"/>
     <col min="9" max="9" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="10" max="17" width="9.140625" customWidth="1"/>
     <col min="18" max="18" width="9.140625" hidden="1" customWidth="1"/>
     <col min="19" max="19" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="10" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A10" s="23" t="s">
+    <row r="1" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B10" s="23"/>
-      <c r="C10" s="23"/>
-      <c r="D10" s="23"/>
-      <c r="E10" s="23"/>
-      <c r="F10" s="23"/>
-      <c r="G10" s="23"/>
-      <c r="H10" s="23"/>
-      <c r="I10" s="23"/>
+      <c r="B1" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="13" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="11" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="12" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A12" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="B12" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="C12" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="D12" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="E12" s="12" t="s">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="F12" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="G12" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="H12" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="I12" s="13" t="s">
-        <v>9</v>
+      <c r="B2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="20">
+        <v>14.3</v>
+      </c>
+      <c r="G2" s="20">
+        <v>11.2</v>
+      </c>
+      <c r="H2" s="16">
+        <v>55000</v>
+      </c>
+      <c r="I2" s="15">
+        <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="14" t="s">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F13" s="20">
+      <c r="D3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="20">
         <v>14.3</v>
       </c>
-      <c r="G13" s="20">
+      <c r="G3" s="20">
         <v>11.2</v>
       </c>
-      <c r="H13" s="16">
+      <c r="H3" s="16">
         <v>55000</v>
       </c>
-      <c r="I13" s="15">
+      <c r="I3" s="15">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="14" t="s">
+    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="C4" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F14" s="20">
+      <c r="D4" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="21">
         <v>14.3</v>
       </c>
-      <c r="G14" s="20">
+      <c r="G4" s="21">
         <v>11.2</v>
       </c>
-      <c r="H14" s="16">
+      <c r="H4" s="18">
         <v>55000</v>
       </c>
-      <c r="I14" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="B15" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C15" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="D15" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="E15" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F15" s="21">
-        <v>14.3</v>
-      </c>
-      <c r="G15" s="21">
-        <v>11.2</v>
-      </c>
-      <c r="H15" s="18">
-        <v>55000</v>
-      </c>
-      <c r="I15" s="19">
+      <c r="I4" s="19">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A10:I10"/>
-  </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.2" right="0.2" top="0.5" bottom="0.25" header="0.05" footer="0.05"/>
   <pageSetup orientation="landscape" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
   <colBreaks count="1" manualBreakCount="1">
     <brk id="9" max="1048575" man="1"/>
   </colBreaks>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
rm dynamic flexcoil insertion for comparison
</commit_message>
<xml_diff>
--- a/app/adp/templates/template.xlsx
+++ b/app/adp/templates/template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\carboni\projects\shupe-carboni\backend\app\adp\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CF5ADE1-C152-4DA9-8490-3E2186568E4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C98437C-9426-4732-9782-95DFC77594C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" tabRatio="856" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" tabRatio="856" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="9-col" sheetId="2" r:id="rId1"/>
@@ -461,7 +461,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="23">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -689,58 +689,6 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -798,7 +746,7 @@
     <xf numFmtId="44" fontId="20" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="20" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -869,21 +817,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="16" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -898,6 +831,15 @@
     </xf>
     <xf numFmtId="0" fontId="19" fillId="33" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="16" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="46">
@@ -970,13 +912,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>3</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>568054</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>184785</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>335052</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>169545</xdr:rowOff>
@@ -1312,103 +1254,93 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B10:U15"/>
+  <dimension ref="B10:S15"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="3" width="34.5703125" customWidth="1"/>
-    <col min="4" max="4" width="16" customWidth="1"/>
-    <col min="5" max="8" width="8.7109375" customWidth="1"/>
-    <col min="9" max="9" width="15.85546875" customWidth="1"/>
-    <col min="10" max="10" width="36.85546875" customWidth="1"/>
-    <col min="11" max="12" width="14.7109375" customWidth="1"/>
-    <col min="13" max="20" width="9.140625" customWidth="1"/>
-    <col min="21" max="21" width="9.140625" hidden="1" customWidth="1"/>
-    <col min="22" max="22" width="0" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="34.5703125" customWidth="1"/>
+    <col min="3" max="3" width="16" customWidth="1"/>
+    <col min="4" max="7" width="8.7109375" customWidth="1"/>
+    <col min="8" max="8" width="15.85546875" customWidth="1"/>
+    <col min="9" max="9" width="36.85546875" customWidth="1"/>
+    <col min="10" max="10" width="14.7109375" customWidth="1"/>
+    <col min="11" max="18" width="9.140625" customWidth="1"/>
+    <col min="19" max="19" width="9.140625" hidden="1" customWidth="1"/>
+    <col min="20" max="20" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="10" spans="2:12" ht="21" x14ac:dyDescent="0.35">
-      <c r="B10" s="30" t="s">
+    <row r="10" spans="2:10" ht="21" x14ac:dyDescent="0.35">
+      <c r="B10" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="C10" s="30"/>
-      <c r="D10" s="30"/>
-      <c r="E10" s="30"/>
-      <c r="F10" s="30"/>
-      <c r="G10" s="30"/>
-      <c r="H10" s="30"/>
-      <c r="I10" s="30"/>
-      <c r="J10" s="30"/>
-      <c r="K10" s="30"/>
-      <c r="L10" s="30"/>
+      <c r="C10" s="25"/>
+      <c r="D10" s="25"/>
+      <c r="E10" s="25"/>
+      <c r="F10" s="25"/>
+      <c r="G10" s="25"/>
+      <c r="H10" s="25"/>
+      <c r="I10" s="25"/>
+      <c r="J10" s="25"/>
     </row>
-    <row r="11" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="12" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B12" s="31"/>
-      <c r="C12" s="32"/>
-      <c r="D12" s="32"/>
-      <c r="E12" s="32"/>
-      <c r="F12" s="32"/>
-      <c r="G12" s="32"/>
-      <c r="H12" s="32"/>
-      <c r="I12" s="32"/>
-      <c r="J12" s="32"/>
-      <c r="K12" s="32"/>
-      <c r="L12" s="33"/>
+    <row r="11" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="12" spans="2:10" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B12" s="26"/>
+      <c r="C12" s="27"/>
+      <c r="D12" s="27"/>
+      <c r="E12" s="27"/>
+      <c r="F12" s="27"/>
+      <c r="G12" s="27"/>
+      <c r="H12" s="27"/>
+      <c r="I12" s="27"/>
+      <c r="J12" s="28"/>
     </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B13" s="4"/>
-      <c r="C13" s="24"/>
+      <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
-      <c r="K13" s="26"/>
-      <c r="L13" s="5"/>
+      <c r="J13" s="29"/>
     </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B14" s="4"/>
-      <c r="C14" s="24"/>
+      <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
-      <c r="J14" s="3"/>
-      <c r="K14" s="27"/>
-      <c r="L14" s="6"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="30"/>
     </row>
-    <row r="15" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="7"/>
-      <c r="C15" s="25"/>
+      <c r="C15" s="8"/>
       <c r="D15" s="8"/>
       <c r="E15" s="8"/>
       <c r="F15" s="8"/>
       <c r="G15" s="8"/>
       <c r="H15" s="8"/>
-      <c r="I15" s="8"/>
-      <c r="J15" s="9"/>
-      <c r="K15" s="28"/>
-      <c r="L15" s="10"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="B10:L10"/>
-    <mergeCell ref="B12:L12"/>
+    <mergeCell ref="B10:J10"/>
+    <mergeCell ref="B12:J12"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.2" right="0.2" top="0.5" bottom="0.25" header="0.05" footer="0.05"/>
   <pageSetup orientation="landscape" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
   <colBreaks count="1" manualBreakCount="1">
-    <brk id="12" max="1048575" man="1"/>
+    <brk id="10" max="1048575" man="1"/>
   </colBreaks>
   <drawing r:id="rId2"/>
 </worksheet>
@@ -1450,7 +1382,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{790636CD-455E-4A76-AE4D-0E945794E185}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
@@ -1482,12 +1414,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="33"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="28"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
@@ -1504,7 +1436,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="29"/>
+      <c r="A3" s="24"/>
       <c r="B3" s="2"/>
       <c r="C3" s="1"/>
       <c r="D3" s="6"/>

</xml_diff>